<commit_message>
redo number of fits, new results in DATA.xlsx
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr showObjects="none" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="60" windowWidth="25000" windowHeight="17300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="160" yWindow="60" windowWidth="18280" windowHeight="17320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="110304" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Element</t>
   </si>
@@ -186,17 +186,26 @@
   </si>
   <si>
     <t>PeakError</t>
+  </si>
+  <si>
+    <t>alternate for 10</t>
+  </si>
+  <si>
+    <t>alternate for -30</t>
+  </si>
+  <si>
+    <t>alternate for -40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -266,7 +275,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -589,14 +598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -721,7 +730,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -729,14 +738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -957,7 +966,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -965,14 +974,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:V30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -1303,46 +1312,46 @@
         <v>800</v>
       </c>
       <c r="C5" s="2">
-        <v>1034.1500000000001</v>
+        <v>542.78499999999997</v>
       </c>
       <c r="D5" s="2">
-        <v>1149.4000000000001</v>
+        <v>20.5443</v>
       </c>
       <c r="E5" s="2">
-        <v>6497.06</v>
+        <v>6483.69</v>
       </c>
       <c r="F5" s="2">
-        <v>74.384100000000004</v>
+        <v>10.114000000000001</v>
       </c>
       <c r="G5" s="2">
-        <v>319.85899999999998</v>
+        <v>248.68299999999999</v>
       </c>
       <c r="H5" s="2">
-        <v>117.879</v>
+        <v>11.1846</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="3"/>
-        <v>20242.861990075355</v>
+        <v>8260.4505931587355</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="11"/>
-        <v>23703.394516886779</v>
+        <v>485.57027782532532</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="4"/>
-        <v>25.303577487594193</v>
+        <v>10.325563241448419</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="5"/>
-        <v>29.629243146108475</v>
+        <v>0.60696284728165661</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" si="6"/>
-        <v>0.5683217219507124</v>
+        <v>0.56716318325188042</v>
       </c>
       <c r="N5" s="12">
         <f t="shared" si="7"/>
-        <v>6.4464587683093575E-3</v>
+        <v>8.8312405594640961E-4</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="8"/>
@@ -1353,19 +1362,19 @@
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="0"/>
-        <v>4.3258438540817665E-24</v>
+        <v>1.7652355406997852E-24</v>
       </c>
       <c r="R5" s="9">
         <f t="shared" ref="R5:R15" si="12">Q5*1E+24</f>
-        <v>4.3258438540817661</v>
+        <v>1.7652355406997851</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="1"/>
-        <v>5.0840234827141762E-24</v>
+        <v>2.0573413246070051E-25</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" si="9"/>
-        <v>5.0840234827141764</v>
+        <v>0.20573413246070049</v>
       </c>
       <c r="U5" s="12">
         <f t="shared" si="2"/>
@@ -1384,46 +1393,46 @@
         <v>1300</v>
       </c>
       <c r="C6" s="2">
-        <v>796.94600000000003</v>
+        <v>497.96100000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>340.02</v>
+        <v>48.900799999999997</v>
       </c>
       <c r="E6" s="2">
-        <v>5070.46</v>
+        <v>5113.43</v>
       </c>
       <c r="F6" s="2">
-        <v>39.8628</v>
+        <v>18.147300000000001</v>
       </c>
       <c r="G6" s="2">
-        <v>346.81900000000002</v>
+        <v>276.863</v>
       </c>
       <c r="H6" s="2">
-        <v>70.671300000000002</v>
+        <v>26.597100000000001</v>
       </c>
       <c r="I6" s="3">
         <f xml:space="preserve"> SQRT(2*3.14159)*G6*C6/40.96</f>
-        <v>16914.594068039365</v>
+        <v>8437.0389426077727</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="11"/>
-        <v>7997.5024617275812</v>
+        <v>1159.0510407707941</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="4"/>
-        <v>13.011226206184126</v>
+        <v>6.4900299558521333</v>
       </c>
       <c r="L6" s="2">
         <f>J6/B6</f>
-        <v>6.1519249705596781</v>
+        <v>0.89157772366984156</v>
       </c>
       <c r="M6" s="12">
         <f t="shared" si="6"/>
-        <v>0.44470382309105411</v>
+        <v>0.44842726421961115</v>
       </c>
       <c r="N6" s="12">
         <f t="shared" si="7"/>
-        <v>3.4555864880120766E-3</v>
+        <v>1.5755734459772977E-3</v>
       </c>
       <c r="O6" s="12">
         <f t="shared" si="8"/>
@@ -1434,23 +1443,23 @@
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="0"/>
-        <v>1.7982736050174836E-24</v>
+        <v>8.9698306527286568E-25</v>
       </c>
       <c r="R6" s="9">
         <f t="shared" si="12"/>
-        <v>1.7982736050174837</v>
+        <v>0.89698306527286564</v>
       </c>
       <c r="S6" s="2">
         <f t="shared" si="1"/>
-        <v>8.6930040499682974E-25</v>
+        <v>1.5275146289312027E-25</v>
       </c>
       <c r="T6" s="9">
         <f t="shared" si="9"/>
-        <v>0.8693004049968297</v>
+        <v>0.15275146289312028</v>
       </c>
       <c r="U6" s="12">
         <f t="shared" si="2"/>
-        <v>3.855616972340576E-2</v>
+        <v>3.8556169723405753E-2</v>
       </c>
       <c r="V6" s="2">
         <f t="shared" si="10"/>
@@ -1465,46 +1474,46 @@
         <v>1500</v>
       </c>
       <c r="C7" s="2">
-        <v>525.89800000000002</v>
+        <v>413.85</v>
       </c>
       <c r="D7" s="2">
-        <v>145.036</v>
+        <v>37.5167</v>
       </c>
       <c r="E7" s="2">
-        <v>4553.45</v>
+        <v>4581.96</v>
       </c>
       <c r="F7" s="2">
-        <v>51.093200000000003</v>
+        <v>15.858700000000001</v>
       </c>
       <c r="G7" s="2">
-        <v>211.125</v>
+        <v>175.90199999999999</v>
       </c>
       <c r="H7" s="2">
-        <v>49.218000000000004</v>
+        <v>19.2317</v>
       </c>
       <c r="I7" s="3">
         <f xml:space="preserve"> SQRT(2*3.14159)*G7*C7/40.96</f>
-        <v>6794.7109214884622</v>
+        <v>4454.9572381897351</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="11"/>
-        <v>2453.6788980251054</v>
+        <v>632.72017937414341</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" si="4"/>
-        <v>4.5298072809923084</v>
+        <v>2.9699714921264899</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" si="5"/>
-        <v>1.6357859320167369</v>
+        <v>0.42181345291609562</v>
       </c>
       <c r="M7" s="12">
         <f t="shared" si="6"/>
-        <v>0.39990381615888532</v>
+        <v>0.40237426778967805</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="7"/>
-        <v>4.4283421079887603E-3</v>
+        <v>1.3774486180996625E-3</v>
       </c>
       <c r="O7" s="12">
         <f t="shared" si="8"/>
@@ -1515,19 +1524,19 @@
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="0"/>
-        <v>5.6965158672061624E-25</v>
+        <v>3.7349248390854974E-25</v>
       </c>
       <c r="R7" s="9">
         <f t="shared" si="12"/>
-        <v>0.56965158672061622</v>
+        <v>0.37349248390854972</v>
       </c>
       <c r="S7" s="2">
         <f t="shared" si="1"/>
-        <v>2.1354926240383177E-25</v>
+        <v>6.5012789452834744E-26</v>
       </c>
       <c r="T7" s="9">
         <f t="shared" si="9"/>
-        <v>0.21354926240383176</v>
+        <v>6.5012789452834743E-2</v>
       </c>
       <c r="U7" s="12">
         <f t="shared" si="2"/>
@@ -1951,46 +1960,46 @@
         <v>600</v>
       </c>
       <c r="C13" s="2">
-        <v>288.54300000000001</v>
+        <v>326.32799999999997</v>
       </c>
       <c r="D13" s="2">
-        <v>58.347900000000003</v>
+        <v>22.5303</v>
       </c>
       <c r="E13" s="2">
-        <v>6142.86</v>
+        <v>6132.27</v>
       </c>
       <c r="F13" s="2">
-        <v>22.539000000000001</v>
+        <v>14.306699999999999</v>
       </c>
       <c r="G13" s="2">
-        <v>195.02600000000001</v>
+        <v>231.851</v>
       </c>
       <c r="H13" s="2">
-        <v>31.0823</v>
+        <v>22.470099999999999</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="3"/>
-        <v>3443.7598556292337</v>
+        <v>4630.1292600338747</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="11"/>
-        <v>886.67016987704778</v>
+        <v>550.95652358657924</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" si="4"/>
-        <v>5.739599759382056</v>
+        <v>7.7168821000564582</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" si="5"/>
-        <v>1.4777836164617464</v>
+        <v>0.91826087264429868</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="6"/>
-        <v>0.53762954490312298</v>
+        <v>0.5367118990676234</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="7"/>
-        <v>1.9559291138798785E-3</v>
+        <v>1.2442265230699476E-3</v>
       </c>
       <c r="O13" s="12">
         <f t="shared" si="8"/>
@@ -2001,19 +2010,19 @@
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="0"/>
-        <v>9.0157233494120838E-25</v>
+        <v>1.2121624686532089E-24</v>
       </c>
       <c r="R13" s="9">
         <f t="shared" si="12"/>
-        <v>0.90157233494120836</v>
+        <v>1.2121624686532089</v>
       </c>
       <c r="S13" s="2">
         <f t="shared" si="1"/>
-        <v>2.4923146795634336E-25</v>
+        <v>1.8890879899478152E-25</v>
       </c>
       <c r="T13" s="9">
         <f t="shared" si="9"/>
-        <v>0.24923146795634335</v>
+        <v>0.18890879899478152</v>
       </c>
       <c r="U13" s="12">
         <f t="shared" si="2"/>
@@ -2179,7 +2188,7 @@
       </c>
       <c r="U15" s="12">
         <f t="shared" si="2"/>
-        <v>3.855616972340576E-2</v>
+        <v>3.8556169723405753E-2</v>
       </c>
       <c r="V15" s="2">
         <f t="shared" si="10"/>
@@ -2343,13 +2352,80 @@
         <v>0.89865600000000001</v>
       </c>
     </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38">
+        <v>110.712</v>
+      </c>
+      <c r="D38">
+        <v>10.232200000000001</v>
+      </c>
+      <c r="E38">
+        <v>7375.32</v>
+      </c>
+      <c r="F38">
+        <v>21.662800000000001</v>
+      </c>
+      <c r="G38">
+        <v>229.49799999999999</v>
+      </c>
+      <c r="H38">
+        <v>27.5611</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39">
+        <v>403.267</v>
+      </c>
+      <c r="D39">
+        <v>37.002800000000001</v>
+      </c>
+      <c r="E39">
+        <v>6156.92</v>
+      </c>
+      <c r="F39">
+        <v>16.875</v>
+      </c>
+      <c r="G39">
+        <v>311.79199999999997</v>
+      </c>
+      <c r="H39">
+        <v>26.801300000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40">
+        <v>464.40100000000001</v>
+      </c>
+      <c r="D40">
+        <v>31.343800000000002</v>
+      </c>
+      <c r="E40">
+        <v>5609.18</v>
+      </c>
+      <c r="F40">
+        <v>18.006799999999998</v>
+      </c>
+      <c r="G40">
+        <v>299.214</v>
+      </c>
+      <c r="H40">
+        <v>22.308700000000002</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>